<commit_message>
4c fine and dandy
</commit_message>
<xml_diff>
--- a/Lab4/4c_tabela.xlsx
+++ b/Lab4/4c_tabela.xlsx
@@ -1,21 +1,80 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="18">
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Qc</t>
+  </si>
+  <si>
+    <t>Qb</t>
+  </si>
+  <si>
+    <t>Qa</t>
+  </si>
+  <si>
+    <t>Wyjście</t>
+  </si>
+  <si>
+    <t>Tabela Karnaugh'a dla Qc</t>
+  </si>
+  <si>
+    <t>(Qc)(Qb)\(Qa)</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Tabela Karnaugh'a dla Qb</t>
+  </si>
+  <si>
+    <t>Tabela Karnaugh'a dla Qa</t>
+  </si>
+  <si>
+    <t>= ~Qa</t>
+  </si>
+  <si>
+    <t>=Qb(~Qa) + (~Qb)Qa = Qb^Qa</t>
+  </si>
+  <si>
+    <t>=Qc(~Qa) + Qa(Qb^Qc)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -23,16 +82,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -40,25 +134,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="3">
+    <cellStyle name="Dobry" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutralny" xfId="2" builtinId="28"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -96,9 +228,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +265,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -168,7 +300,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -341,13 +473,422 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="12.77734375" customWidth="1"/>
+    <col min="8" max="8" width="2.44140625" customWidth="1"/>
+    <col min="9" max="9" width="2.5546875" customWidth="1"/>
+    <col min="11" max="11" width="13" customWidth="1"/>
+    <col min="12" max="12" width="2.44140625" customWidth="1"/>
+    <col min="13" max="13" width="2.5546875" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" customWidth="1"/>
+    <col min="16" max="16" width="2.6640625" customWidth="1"/>
+    <col min="17" max="17" width="3.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="7"/>
+      <c r="K3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" s="7"/>
+      <c r="O3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="R3" s="4"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4" s="4"/>
+      <c r="O4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="R4" s="4"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" s="4"/>
+      <c r="O5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="R5" s="4"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N6" s="4"/>
+      <c r="O6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="R6" s="4"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="N7" s="4"/>
+      <c r="O7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="R7" s="4"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="P9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>